<commit_message>
Added template for our presentation. And documentation.
</commit_message>
<xml_diff>
--- a/Info.xlsx
+++ b/Info.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Most important C\Учёбушка С\CV camp\Workout-check\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF65526D-F110-412F-B766-8BBC8888A993}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="10770" xr2:uid="{DEF9E440-DE11-45EF-9C01-A8856582795E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="10770"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,37 +25,95 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>База для сравнения</t>
-  </si>
-  <si>
-    <t>Наклон головы влево-вправо</t>
-  </si>
-  <si>
-    <t>Поворот головы влево-вправо</t>
-  </si>
-  <si>
-    <t>Наклон головы вперёд-назад</t>
-  </si>
-  <si>
-    <t>Задачи для решения</t>
-  </si>
-  <si>
-    <t>Понять по каким параметрам оценивать</t>
-  </si>
-  <si>
-    <t>база для сравнения</t>
-  </si>
-  <si>
-    <t>реализация "трекера"</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>Упражнение "Наклон головы вправо-влево"</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>Упражнение "Наклон головы вперёд-назад"</t>
+  </si>
+  <si>
+    <t>Упражнение "Поворот головы вправо-влево"</t>
+  </si>
+  <si>
+    <t>Реализованные 
+упражнения</t>
+  </si>
+  <si>
+    <t>Параметры оценки
+ Упражнения №1</t>
+  </si>
+  <si>
+    <t>Параметры оценки
+ Упражнения №2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. </t>
+  </si>
+  <si>
+    <t>Сравнение предыдущих значений крайних точек
+ задетектированного лица (left-top, right-bottom) с последующими.</t>
+  </si>
+  <si>
+    <t>Создан класс comparison - наследник класса ComparatorTemplate,
+ в котором реализована вирутальная функция Compare_ex3.</t>
+  </si>
+  <si>
+    <t>Параметры оценки
+ Упражнения №3</t>
+  </si>
+  <si>
+    <t>Создан класс comparison - наследник класса ComparatorTemplate,
+ в котором реализована вирутальная функция Compare_ex2.</t>
+  </si>
+  <si>
+    <t>В классе Compare_ex2, непосредственно, происходит сравнение точек: 
+отклонение точек left-right должно быть минимальным при выполнении упражнения,
+ а отклонение точек top-bottom -должно отличаться от предыдущих их положений. 
+Таким образом, при правильном выполнении задания оба эти условия должны быть соблюдены, 
+иначе - выходу из программы.</t>
+  </si>
+  <si>
+    <t>Сравнение положений лица при поворотах в одну и другую сторону.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">В классе Compare_ex3, непосредственно, происходит сравнение площадей задетектированного прямоугольника: 
+Максимальая площадь прямоугольника - в начальный и конечный моменты занятия, когда лицо находится в положении "анфас". Далее - при поворотах головы - площадь данного прямоугольника уменьшается, приобретая некий минимум, запоминаем этот минимум. То же самое происходит при повороте в другую сторону. 
+Последним шагом является сравнение этих двух минимумов, если их разность(отклонение) плюс-минус равно - упражнение выполнено правильно, иначе - выход из программы.
+</t>
+  </si>
+  <si>
+    <t>P.S.: все движения (упражнения) должны выполняться с равной скоростью(равномерно), иначе - 
+упражнение вредит вашему здоровью - а значит, выполнено неправильно(выход из программы)</t>
+  </si>
+  <si>
+    <t>Первоначально, для детектирования лица, был использован метод Каскады Хаара. Его суть заключалась в подключении файла, местоположение которого - "..\opencv\opencv\sources\data\haarcascades\haarcascade_frontalface_alt.xml", и дальнейшее его использование при посике лица на кадре.</t>
+  </si>
+  <si>
+    <t>Плюсы: короткий и понятный код. Работает.</t>
+  </si>
+  <si>
+    <t>Минусы: медленно работает, неэффективно.</t>
+  </si>
+  <si>
+    <t>Реализация метода
+ Хаар</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -87,14 +139,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -156,7 +288,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -208,7 +340,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -402,89 +534,168 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51917BC1-0E18-4F34-959D-91E85264A1A0}">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A7"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" customWidth="1"/>
+    <col min="3" max="4" width="92.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="5"/>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="8"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="8"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:3" ht="30">
+      <c r="A9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30">
+      <c r="A10" s="8"/>
+      <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6">
+      <c r="C10" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="90">
+      <c r="A11" s="8"/>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30">
+      <c r="A14" s="8"/>
+      <c r="B14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
+      <c r="C14" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="135">
+      <c r="A15" s="8"/>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="33" customHeight="1">
+      <c r="C17" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="60">
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="B19:B21"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A19:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>